<commit_message>
atualizei lista do excell do professor, do doc TODO
</commit_message>
<xml_diff>
--- a/Recursos/2014-10-17 Checklist Avaliacao BDA.xlsx
+++ b/Recursos/2014-10-17 Checklist Avaliacao BDA.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25007"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27715"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/joaopaulobrasdelgado/Desktop/Mestrado CM/Base de Dados Avançadas/Oficina-online/Recursos/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="16340" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="28800" windowHeight="16560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,11 @@
   <definedNames>
     <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$I$43</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -220,7 +228,6 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <charset val="128"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -640,6 +647,42 @@
     <xf numFmtId="9" fontId="8" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -655,6 +698,39 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="164" fontId="7" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -672,75 +748,6 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="110">
@@ -857,6 +864,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -1187,11 +1199,11 @@
   </sheetPr>
   <dimension ref="A1:I43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:I2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="7.83203125" customWidth="1"/>
     <col min="2" max="2" width="5.6640625" bestFit="1" customWidth="1"/>
@@ -1203,33 +1215,33 @@
     <col min="9" max="9" width="9.1640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="20">
-      <c r="A1" s="58" t="s">
+    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.25">
+      <c r="A1" s="36" t="s">
         <v>60</v>
       </c>
-      <c r="B1" s="59"/>
-      <c r="C1" s="59"/>
-      <c r="D1" s="59"/>
-      <c r="E1" s="59"/>
-      <c r="F1" s="59"/>
-      <c r="G1" s="59"/>
-      <c r="H1" s="59"/>
-      <c r="I1" s="59"/>
-    </row>
-    <row r="2" spans="1:9" ht="18">
-      <c r="A2" s="61" t="s">
+      <c r="B1" s="37"/>
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="37"/>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37"/>
+    </row>
+    <row r="2" spans="1:9" ht="19" x14ac:dyDescent="0.25">
+      <c r="A2" s="39" t="s">
         <v>38</v>
       </c>
-      <c r="B2" s="61"/>
-      <c r="C2" s="61"/>
-      <c r="D2" s="61"/>
-      <c r="E2" s="61"/>
-      <c r="F2" s="61"/>
-      <c r="G2" s="61"/>
-      <c r="H2" s="61"/>
-      <c r="I2" s="61"/>
-    </row>
-    <row r="3" spans="1:9">
+      <c r="B2" s="39"/>
+      <c r="C2" s="39"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
+      <c r="G2" s="39"/>
+      <c r="H2" s="39"/>
+      <c r="I2" s="39"/>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
       <c r="B3" s="1"/>
       <c r="C3" s="1"/>
@@ -1238,18 +1250,18 @@
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
-    <row r="4" spans="1:9">
-      <c r="A4" s="50" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A4" s="28" t="s">
         <v>13</v>
       </c>
-      <c r="B4" s="51"/>
+      <c r="B4" s="29"/>
       <c r="C4" s="3"/>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
       <c r="B5" s="1"/>
       <c r="C5" s="1"/>
@@ -1258,57 +1270,57 @@
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
-    <row r="6" spans="1:9">
-      <c r="A6" s="50" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A6" s="28" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="51"/>
+      <c r="B6" s="29"/>
       <c r="C6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D6" s="60" t="s">
+      <c r="D6" s="38" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="60"/>
-      <c r="F6" s="60"/>
-      <c r="G6" s="60"/>
-      <c r="H6" s="60"/>
-      <c r="I6" s="60"/>
-    </row>
-    <row r="7" spans="1:9">
-      <c r="A7" s="52"/>
-      <c r="B7" s="53"/>
+      <c r="E6" s="38"/>
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A7" s="30"/>
+      <c r="B7" s="31"/>
       <c r="C7" s="2"/>
-      <c r="D7" s="60"/>
-      <c r="E7" s="60"/>
-      <c r="F7" s="60"/>
-      <c r="G7" s="60"/>
-      <c r="H7" s="60"/>
-      <c r="I7" s="60"/>
-    </row>
-    <row r="8" spans="1:9">
-      <c r="A8" s="54"/>
-      <c r="B8" s="55"/>
+      <c r="D7" s="38"/>
+      <c r="E7" s="38"/>
+      <c r="F7" s="38"/>
+      <c r="G7" s="38"/>
+      <c r="H7" s="38"/>
+      <c r="I7" s="38"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A8" s="32"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="2"/>
-      <c r="D8" s="60"/>
-      <c r="E8" s="60"/>
-      <c r="F8" s="60"/>
-      <c r="G8" s="60"/>
-      <c r="H8" s="60"/>
-      <c r="I8" s="60"/>
-    </row>
-    <row r="9" spans="1:9">
-      <c r="A9" s="56"/>
-      <c r="B9" s="57"/>
+      <c r="D8" s="38"/>
+      <c r="E8" s="38"/>
+      <c r="F8" s="38"/>
+      <c r="G8" s="38"/>
+      <c r="H8" s="38"/>
+      <c r="I8" s="38"/>
+    </row>
+    <row r="9" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A9" s="34"/>
+      <c r="B9" s="35"/>
       <c r="C9" s="3"/>
-      <c r="D9" s="60"/>
-      <c r="E9" s="60"/>
-      <c r="F9" s="60"/>
-      <c r="G9" s="60"/>
-      <c r="H9" s="60"/>
-      <c r="I9" s="60"/>
-    </row>
-    <row r="10" spans="1:9">
+      <c r="D9" s="38"/>
+      <c r="E9" s="38"/>
+      <c r="F9" s="38"/>
+      <c r="G9" s="38"/>
+      <c r="H9" s="38"/>
+      <c r="I9" s="38"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A10" s="4"/>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -1317,7 +1329,7 @@
       <c r="F10" s="4"/>
       <c r="G10" s="4"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" s="4"/>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1326,7 +1338,7 @@
       <c r="F11" s="4"/>
       <c r="G11" s="4"/>
     </row>
-    <row r="12" spans="1:9" ht="30">
+    <row r="12" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A12" s="10" t="s">
         <v>26</v>
       </c>
@@ -1355,15 +1367,15 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" ht="15" customHeight="1">
-      <c r="A13" s="39">
+    <row r="13" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A13" s="45">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="B13" s="42">
+      <c r="B13" s="48">
         <f>A13*20</f>
         <v>1.5</v>
       </c>
-      <c r="C13" s="47" t="s">
+      <c r="C13" s="51" t="s">
         <v>1</v>
       </c>
       <c r="D13" s="5" t="s">
@@ -1375,7 +1387,7 @@
       <c r="F13" s="7">
         <v>0</v>
       </c>
-      <c r="G13" s="31">
+      <c r="G13" s="43">
         <f>$A13*(F17*50%+IF(OR(F16="S",F16="s"),1,0)*20%+IF(OR(F15="S",F15="s"),1,0)*10%+IF(F13&gt;5,5,F13)/5*10%+IF(F14&gt;3,3,F14)/3*10%)*20</f>
         <v>0</v>
       </c>
@@ -1383,15 +1395,15 @@
         <f t="shared" ref="H13:H23" si="0">F13</f>
         <v>0</v>
       </c>
-      <c r="I13" s="31">
+      <c r="I13" s="43">
         <f>$A13*(H17*50%+IF(OR(H16="S",H16="s"),1,0)*20%+IF(OR(H15="S",H15="s"),1,0)*10%+IF(H13&gt;5,5,H13)/5*10%+IF(H14&gt;3,3,H14)/3*10%)*20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:9" ht="15" customHeight="1">
-      <c r="A14" s="40"/>
-      <c r="B14" s="43"/>
-      <c r="C14" s="48"/>
+    <row r="14" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A14" s="46"/>
+      <c r="B14" s="49"/>
+      <c r="C14" s="52"/>
       <c r="D14" s="5" t="s">
         <v>52</v>
       </c>
@@ -1401,17 +1413,17 @@
       <c r="F14" s="7">
         <v>0</v>
       </c>
-      <c r="G14" s="46"/>
+      <c r="G14" s="54"/>
       <c r="H14" s="18">
         <f>F14</f>
         <v>0</v>
       </c>
-      <c r="I14" s="46"/>
-    </row>
-    <row r="15" spans="1:9">
-      <c r="A15" s="40"/>
-      <c r="B15" s="43"/>
-      <c r="C15" s="48"/>
+      <c r="I14" s="54"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A15" s="46"/>
+      <c r="B15" s="49"/>
+      <c r="C15" s="52"/>
       <c r="D15" s="5" t="s">
         <v>57</v>
       </c>
@@ -1421,17 +1433,17 @@
       <c r="F15" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G15" s="46"/>
+      <c r="G15" s="54"/>
       <c r="H15" s="18" t="str">
         <f t="shared" si="0"/>
         <v>n</v>
       </c>
-      <c r="I15" s="46"/>
-    </row>
-    <row r="16" spans="1:9">
-      <c r="A16" s="40"/>
-      <c r="B16" s="43"/>
-      <c r="C16" s="48"/>
+      <c r="I15" s="54"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A16" s="46"/>
+      <c r="B16" s="49"/>
+      <c r="C16" s="52"/>
       <c r="D16" s="5" t="s">
         <v>58</v>
       </c>
@@ -1441,17 +1453,17 @@
       <c r="F16" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G16" s="46"/>
+      <c r="G16" s="54"/>
       <c r="H16" s="18" t="str">
         <f t="shared" si="0"/>
         <v>n</v>
       </c>
-      <c r="I16" s="46"/>
-    </row>
-    <row r="17" spans="1:9">
-      <c r="A17" s="41"/>
-      <c r="B17" s="44"/>
-      <c r="C17" s="49"/>
+      <c r="I16" s="54"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A17" s="47"/>
+      <c r="B17" s="50"/>
+      <c r="C17" s="53"/>
       <c r="D17" s="5" t="s">
         <v>59</v>
       </c>
@@ -1461,22 +1473,22 @@
       <c r="F17" s="8">
         <v>0</v>
       </c>
-      <c r="G17" s="32"/>
+      <c r="G17" s="44"/>
       <c r="H17" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I17" s="32"/>
-    </row>
-    <row r="18" spans="1:9">
-      <c r="A18" s="28">
+      <c r="I17" s="44"/>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A18" s="40">
         <v>2.5000000000000001E-2</v>
       </c>
-      <c r="B18" s="29">
+      <c r="B18" s="41">
         <f>A18*20</f>
         <v>0.5</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="55" t="s">
         <v>0</v>
       </c>
       <c r="D18" s="5" t="s">
@@ -1488,7 +1500,7 @@
       <c r="F18" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G18" s="31">
+      <c r="G18" s="43">
         <f>$A18*(F19*60%+IF(OR(F18="S",F18="s"),1,0)*40%)*20</f>
         <v>0</v>
       </c>
@@ -1496,15 +1508,15 @@
         <f t="shared" si="0"/>
         <v>n</v>
       </c>
-      <c r="I18" s="31">
+      <c r="I18" s="43">
         <f>$A18*(H19*60%+IF(OR(H18="S",H18="s"),1,0)*40%)*20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:9" ht="30">
-      <c r="A19" s="28"/>
-      <c r="B19" s="29"/>
-      <c r="C19" s="45"/>
+    <row r="19" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A19" s="40"/>
+      <c r="B19" s="41"/>
+      <c r="C19" s="55"/>
       <c r="D19" s="5" t="s">
         <v>14</v>
       </c>
@@ -1514,14 +1526,14 @@
       <c r="F19" s="8">
         <v>0</v>
       </c>
-      <c r="G19" s="32"/>
+      <c r="G19" s="44"/>
       <c r="H19" s="14">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I19" s="32"/>
-    </row>
-    <row r="20" spans="1:9" ht="30">
+      <c r="I19" s="44"/>
+    </row>
+    <row r="20" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A20" s="20">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -1554,15 +1566,15 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:9" ht="15" customHeight="1">
-      <c r="A21" s="39">
+    <row r="21" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A21" s="45">
         <v>7.4999999999999997E-2</v>
       </c>
-      <c r="B21" s="42">
+      <c r="B21" s="48">
         <f>A21*20</f>
         <v>1.5</v>
       </c>
-      <c r="C21" s="47" t="s">
+      <c r="C21" s="51" t="s">
         <v>51</v>
       </c>
       <c r="D21" s="5" t="s">
@@ -1574,7 +1586,7 @@
       <c r="F21" s="7">
         <v>0</v>
       </c>
-      <c r="G21" s="31">
+      <c r="G21" s="43">
         <f>$A21*(IF(F27&gt;1,1,F27)*10%+IF(SUM(F24:F26)&gt;12,12,SUM(F24:F26))/12*60%+IF(F23&gt;2,2,F23)/2*10%+IF(F22&gt;2,2,F22)/2*10%+IF(F21&gt;2,2,F21)/2*10%)*20</f>
         <v>0</v>
       </c>
@@ -1582,15 +1594,15 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I21" s="31">
+      <c r="I21" s="43">
         <f>$A21*(IF(H27&gt;1,1,H27)*10%+IF(SUM(H24:H26)&gt;12,12,SUM(H24:H26))/12*60%+IF(H23&gt;2,2,H23)/2*10%+IF(H22&gt;2,2,H22)/2*10%+IF(H21&gt;2,2,H21)/2*10%)*20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:9">
-      <c r="A22" s="40"/>
-      <c r="B22" s="43"/>
-      <c r="C22" s="48"/>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="46"/>
+      <c r="B22" s="49"/>
+      <c r="C22" s="52"/>
       <c r="D22" s="5" t="s">
         <v>22</v>
       </c>
@@ -1600,17 +1612,17 @@
       <c r="F22" s="7">
         <v>0</v>
       </c>
-      <c r="G22" s="46"/>
+      <c r="G22" s="54"/>
       <c r="H22" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I22" s="46"/>
-    </row>
-    <row r="23" spans="1:9">
-      <c r="A23" s="40"/>
-      <c r="B23" s="43"/>
-      <c r="C23" s="48"/>
+      <c r="I22" s="54"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="46"/>
+      <c r="B23" s="49"/>
+      <c r="C23" s="52"/>
       <c r="D23" s="5" t="s">
         <v>21</v>
       </c>
@@ -1620,17 +1632,17 @@
       <c r="F23" s="7">
         <v>0</v>
       </c>
-      <c r="G23" s="46"/>
+      <c r="G23" s="54"/>
       <c r="H23" s="18">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="I23" s="46"/>
-    </row>
-    <row r="24" spans="1:9">
-      <c r="A24" s="40"/>
-      <c r="B24" s="43"/>
-      <c r="C24" s="48"/>
+      <c r="I23" s="54"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="46"/>
+      <c r="B24" s="49"/>
+      <c r="C24" s="52"/>
       <c r="D24" s="5" t="s">
         <v>47</v>
       </c>
@@ -1640,17 +1652,17 @@
       <c r="F24" s="7">
         <v>0</v>
       </c>
-      <c r="G24" s="46"/>
+      <c r="G24" s="54"/>
       <c r="H24" s="11">
         <f>F24</f>
         <v>0</v>
       </c>
-      <c r="I24" s="46"/>
-    </row>
-    <row r="25" spans="1:9">
-      <c r="A25" s="40"/>
-      <c r="B25" s="43"/>
-      <c r="C25" s="48"/>
+      <c r="I24" s="54"/>
+    </row>
+    <row r="25" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A25" s="46"/>
+      <c r="B25" s="49"/>
+      <c r="C25" s="52"/>
       <c r="D25" s="5" t="s">
         <v>48</v>
       </c>
@@ -1660,17 +1672,17 @@
       <c r="F25" s="7">
         <v>0</v>
       </c>
-      <c r="G25" s="46"/>
+      <c r="G25" s="54"/>
       <c r="H25" s="11">
         <f t="shared" ref="H25:H27" si="1">F25</f>
         <v>0</v>
       </c>
-      <c r="I25" s="46"/>
-    </row>
-    <row r="26" spans="1:9">
-      <c r="A26" s="40"/>
-      <c r="B26" s="43"/>
-      <c r="C26" s="48"/>
+      <c r="I25" s="54"/>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="46"/>
+      <c r="B26" s="49"/>
+      <c r="C26" s="52"/>
       <c r="D26" s="5" t="s">
         <v>49</v>
       </c>
@@ -1680,17 +1692,17 @@
       <c r="F26" s="7">
         <v>0</v>
       </c>
-      <c r="G26" s="46"/>
+      <c r="G26" s="54"/>
       <c r="H26" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I26" s="46"/>
-    </row>
-    <row r="27" spans="1:9">
-      <c r="A27" s="41"/>
-      <c r="B27" s="44"/>
-      <c r="C27" s="49"/>
+      <c r="I26" s="54"/>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A27" s="47"/>
+      <c r="B27" s="50"/>
+      <c r="C27" s="53"/>
       <c r="D27" s="5" t="s">
         <v>50</v>
       </c>
@@ -1700,22 +1712,22 @@
       <c r="F27" s="7">
         <v>0</v>
       </c>
-      <c r="G27" s="32"/>
+      <c r="G27" s="44"/>
       <c r="H27" s="11">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I27" s="32"/>
-    </row>
-    <row r="28" spans="1:9" ht="15" customHeight="1">
-      <c r="A28" s="39">
+      <c r="I27" s="44"/>
+    </row>
+    <row r="28" spans="1:9" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A28" s="45">
         <v>0.2</v>
       </c>
-      <c r="B28" s="42">
+      <c r="B28" s="48">
         <f>A28*20</f>
         <v>4</v>
       </c>
-      <c r="C28" s="47" t="s">
+      <c r="C28" s="51" t="s">
         <v>3</v>
       </c>
       <c r="D28" s="5" t="s">
@@ -1727,7 +1739,7 @@
       <c r="F28" s="7">
         <v>0</v>
       </c>
-      <c r="G28" s="31">
+      <c r="G28" s="43">
         <f>$A28*(F31*40%+F30*40%+IF(F29&gt;3,3,F29)/3*10%+IF(F28&gt;3,3,F28)/3*10%)*20</f>
         <v>0</v>
       </c>
@@ -1735,15 +1747,15 @@
         <f t="shared" ref="H28:H31" si="2">F28</f>
         <v>0</v>
       </c>
-      <c r="I28" s="31">
+      <c r="I28" s="43">
         <f>$A28*(H31*40%+H30*40%+IF(H29&gt;3,3,H29)/3*10%+IF(H28&gt;3,3,H28)/3*10%)*20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:9">
-      <c r="A29" s="40"/>
-      <c r="B29" s="43"/>
-      <c r="C29" s="48"/>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A29" s="46"/>
+      <c r="B29" s="49"/>
+      <c r="C29" s="52"/>
       <c r="D29" s="5" t="s">
         <v>19</v>
       </c>
@@ -1753,17 +1765,17 @@
       <c r="F29" s="7">
         <v>0</v>
       </c>
-      <c r="G29" s="46"/>
+      <c r="G29" s="54"/>
       <c r="H29" s="18">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I29" s="46"/>
-    </row>
-    <row r="30" spans="1:9" ht="30">
-      <c r="A30" s="40"/>
-      <c r="B30" s="43"/>
-      <c r="C30" s="48"/>
+      <c r="I29" s="54"/>
+    </row>
+    <row r="30" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A30" s="46"/>
+      <c r="B30" s="49"/>
+      <c r="C30" s="52"/>
       <c r="D30" s="5" t="s">
         <v>54</v>
       </c>
@@ -1773,17 +1785,17 @@
       <c r="F30" s="8">
         <v>0</v>
       </c>
-      <c r="G30" s="46"/>
+      <c r="G30" s="54"/>
       <c r="H30" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I30" s="46"/>
-    </row>
-    <row r="31" spans="1:9" ht="30">
-      <c r="A31" s="41"/>
-      <c r="B31" s="44"/>
-      <c r="C31" s="49"/>
+      <c r="I30" s="54"/>
+    </row>
+    <row r="31" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A31" s="47"/>
+      <c r="B31" s="50"/>
+      <c r="C31" s="53"/>
       <c r="D31" s="5" t="s">
         <v>55</v>
       </c>
@@ -1793,22 +1805,22 @@
       <c r="F31" s="8">
         <v>0</v>
       </c>
-      <c r="G31" s="32"/>
+      <c r="G31" s="44"/>
       <c r="H31" s="14">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="I31" s="32"/>
-    </row>
-    <row r="32" spans="1:9">
-      <c r="A32" s="39">
+      <c r="I31" s="44"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A32" s="45">
         <v>0.1</v>
       </c>
-      <c r="B32" s="42">
+      <c r="B32" s="48">
         <f>A32*20</f>
         <v>2</v>
       </c>
-      <c r="C32" s="45" t="s">
+      <c r="C32" s="55" t="s">
         <v>4</v>
       </c>
       <c r="D32" s="5" t="s">
@@ -1820,7 +1832,7 @@
       <c r="F32" s="7">
         <v>0</v>
       </c>
-      <c r="G32" s="31">
+      <c r="G32" s="43">
         <f>$A32*(F34*50%+F33*40%+IF(F32&gt;2,2,F32)/2*10%)*20</f>
         <v>0</v>
       </c>
@@ -1828,15 +1840,15 @@
         <f t="shared" ref="H32:H34" si="3">F32</f>
         <v>0</v>
       </c>
-      <c r="I32" s="31">
+      <c r="I32" s="43">
         <f>$A32*(H34*50%+H33*40%+IF(H32&gt;2,2,H32)/2*10%)*20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:9">
-      <c r="A33" s="40"/>
-      <c r="B33" s="43"/>
-      <c r="C33" s="45"/>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A33" s="46"/>
+      <c r="B33" s="49"/>
+      <c r="C33" s="55"/>
       <c r="D33" s="5" t="s">
         <v>41</v>
       </c>
@@ -1846,17 +1858,17 @@
       <c r="F33" s="8">
         <v>0</v>
       </c>
-      <c r="G33" s="46"/>
+      <c r="G33" s="54"/>
       <c r="H33" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I33" s="46"/>
-    </row>
-    <row r="34" spans="1:9" ht="30">
-      <c r="A34" s="41"/>
-      <c r="B34" s="44"/>
-      <c r="C34" s="45"/>
+      <c r="I33" s="54"/>
+    </row>
+    <row r="34" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A34" s="47"/>
+      <c r="B34" s="50"/>
+      <c r="C34" s="55"/>
       <c r="D34" s="5" t="s">
         <v>42</v>
       </c>
@@ -1866,22 +1878,22 @@
       <c r="F34" s="8">
         <v>0</v>
       </c>
-      <c r="G34" s="32"/>
+      <c r="G34" s="44"/>
       <c r="H34" s="14">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="I34" s="32"/>
-    </row>
-    <row r="35" spans="1:9">
-      <c r="A35" s="33">
+      <c r="I34" s="44"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A35" s="56">
         <v>0.1</v>
       </c>
-      <c r="B35" s="35">
+      <c r="B35" s="58">
         <f>A35*20</f>
         <v>2</v>
       </c>
-      <c r="C35" s="37" t="s">
+      <c r="C35" s="60" t="s">
         <v>39</v>
       </c>
       <c r="D35" s="22" t="s">
@@ -1893,7 +1905,7 @@
       <c r="F35" s="26">
         <v>0</v>
       </c>
-      <c r="G35" s="35">
+      <c r="G35" s="58">
         <f>$A32*(F36*50%+F35*50%)*20</f>
         <v>0</v>
       </c>
@@ -1901,15 +1913,15 @@
         <f>F35</f>
         <v>0</v>
       </c>
-      <c r="I35" s="35">
+      <c r="I35" s="58">
         <f>$A32*(H36*50%+H35*50%)*20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:9">
-      <c r="A36" s="34"/>
-      <c r="B36" s="36"/>
-      <c r="C36" s="38"/>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A36" s="57"/>
+      <c r="B36" s="59"/>
+      <c r="C36" s="61"/>
       <c r="D36" s="24" t="s">
         <v>46</v>
       </c>
@@ -1919,22 +1931,22 @@
       <c r="F36" s="26">
         <v>0</v>
       </c>
-      <c r="G36" s="36"/>
+      <c r="G36" s="59"/>
       <c r="H36" s="27">
         <f>F36</f>
         <v>0</v>
       </c>
-      <c r="I36" s="36"/>
-    </row>
-    <row r="37" spans="1:9" ht="30">
-      <c r="A37" s="28">
+      <c r="I36" s="59"/>
+    </row>
+    <row r="37" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A37" s="40">
         <v>0.1</v>
       </c>
-      <c r="B37" s="29">
+      <c r="B37" s="41">
         <f>A37*20</f>
         <v>2</v>
       </c>
-      <c r="C37" s="30" t="s">
+      <c r="C37" s="42" t="s">
         <v>5</v>
       </c>
       <c r="D37" s="5" t="s">
@@ -1946,7 +1958,7 @@
       <c r="F37" s="8">
         <v>0</v>
       </c>
-      <c r="G37" s="31">
+      <c r="G37" s="43">
         <f>$A37*(F37*25%+IF(OR(F38="S",F38="s"),1,0)*75%)*20</f>
         <v>0</v>
       </c>
@@ -1954,15 +1966,15 @@
         <f>F37</f>
         <v>0</v>
       </c>
-      <c r="I37" s="31">
+      <c r="I37" s="43">
         <f>$A37*(H37*25%+IF(OR(H38="S",H38="s"),1,0)*75%)*20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:9" ht="30">
-      <c r="A38" s="28"/>
-      <c r="B38" s="29"/>
-      <c r="C38" s="30"/>
+    <row r="38" spans="1:9" ht="32" x14ac:dyDescent="0.2">
+      <c r="A38" s="40"/>
+      <c r="B38" s="41"/>
+      <c r="C38" s="42"/>
       <c r="D38" s="5" t="s">
         <v>18</v>
       </c>
@@ -1972,22 +1984,22 @@
       <c r="F38" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G38" s="32"/>
+      <c r="G38" s="44"/>
       <c r="H38" s="18" t="str">
         <f t="shared" ref="H38" si="4">F38</f>
         <v>n</v>
       </c>
-      <c r="I38" s="32"/>
-    </row>
-    <row r="39" spans="1:9">
-      <c r="A39" s="28">
+      <c r="I38" s="44"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A39" s="40">
         <v>0.2</v>
       </c>
-      <c r="B39" s="29">
+      <c r="B39" s="41">
         <f>A39*20</f>
         <v>4</v>
       </c>
-      <c r="C39" s="30" t="s">
+      <c r="C39" s="42" t="s">
         <v>40</v>
       </c>
       <c r="D39" s="5" t="s">
@@ -1999,7 +2011,7 @@
       <c r="F39" s="8">
         <v>0</v>
       </c>
-      <c r="G39" s="31">
+      <c r="G39" s="43">
         <f>$A39*(F39*50%+IF(OR(F40="S",F40="s"),1,0)*50%)*20</f>
         <v>0</v>
       </c>
@@ -2007,15 +2019,15 @@
         <f>F39</f>
         <v>0</v>
       </c>
-      <c r="I39" s="31">
+      <c r="I39" s="43">
         <f>$A39*(H39*50%+IF(OR(H40="S",H40="s"),1,0)*50%)*20</f>
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:9">
-      <c r="A40" s="28"/>
-      <c r="B40" s="29"/>
-      <c r="C40" s="30"/>
+    <row r="40" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A40" s="40"/>
+      <c r="B40" s="41"/>
+      <c r="C40" s="42"/>
       <c r="D40" s="5" t="s">
         <v>45</v>
       </c>
@@ -2025,14 +2037,14 @@
       <c r="F40" s="7" t="s">
         <v>37</v>
       </c>
-      <c r="G40" s="32"/>
+      <c r="G40" s="44"/>
       <c r="H40" s="18" t="str">
         <f t="shared" ref="H40" si="5">F40</f>
         <v>n</v>
       </c>
-      <c r="I40" s="32"/>
-    </row>
-    <row r="41" spans="1:9">
+      <c r="I40" s="44"/>
+    </row>
+    <row r="41" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A41" s="20">
         <v>2.5000000000000001E-2</v>
       </c>
@@ -2065,7 +2077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:9" ht="45">
+    <row r="42" spans="1:9" ht="48" x14ac:dyDescent="0.2">
       <c r="A42" s="20">
         <v>7.4999999999999997E-2</v>
       </c>
@@ -2098,7 +2110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:9" ht="30">
+    <row r="43" spans="1:9" ht="32" x14ac:dyDescent="0.2">
       <c r="A43" s="12">
         <f>SUM(A7:A42)</f>
         <v>0.99999999999999989</v>
@@ -2124,6 +2136,46 @@
     </row>
   </sheetData>
   <mergeCells count="49">
+    <mergeCell ref="A39:A40"/>
+    <mergeCell ref="B39:B40"/>
+    <mergeCell ref="C39:C40"/>
+    <mergeCell ref="G39:G40"/>
+    <mergeCell ref="I39:I40"/>
+    <mergeCell ref="A35:A36"/>
+    <mergeCell ref="B35:B36"/>
+    <mergeCell ref="C35:C36"/>
+    <mergeCell ref="G35:G36"/>
+    <mergeCell ref="I35:I36"/>
+    <mergeCell ref="A32:A34"/>
+    <mergeCell ref="B32:B34"/>
+    <mergeCell ref="C32:C34"/>
+    <mergeCell ref="G32:G34"/>
+    <mergeCell ref="I32:I34"/>
+    <mergeCell ref="C28:C31"/>
+    <mergeCell ref="B28:B31"/>
+    <mergeCell ref="A28:A31"/>
+    <mergeCell ref="G28:G31"/>
+    <mergeCell ref="I28:I31"/>
+    <mergeCell ref="C21:C27"/>
+    <mergeCell ref="B21:B27"/>
+    <mergeCell ref="A21:A27"/>
+    <mergeCell ref="G21:G27"/>
+    <mergeCell ref="I21:I27"/>
+    <mergeCell ref="A18:A19"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="C18:C19"/>
+    <mergeCell ref="G18:G19"/>
+    <mergeCell ref="I18:I19"/>
+    <mergeCell ref="A13:A17"/>
+    <mergeCell ref="B13:B17"/>
+    <mergeCell ref="C13:C17"/>
+    <mergeCell ref="G13:G17"/>
+    <mergeCell ref="I13:I17"/>
+    <mergeCell ref="A37:A38"/>
+    <mergeCell ref="B37:B38"/>
+    <mergeCell ref="C37:C38"/>
+    <mergeCell ref="G37:G38"/>
+    <mergeCell ref="I37:I38"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A6:B6"/>
     <mergeCell ref="A7:B9"/>
@@ -2133,54 +2185,9 @@
     <mergeCell ref="D8:I8"/>
     <mergeCell ref="D9:I9"/>
     <mergeCell ref="A2:I2"/>
-    <mergeCell ref="A37:A38"/>
-    <mergeCell ref="B37:B38"/>
-    <mergeCell ref="C37:C38"/>
-    <mergeCell ref="G37:G38"/>
-    <mergeCell ref="I37:I38"/>
-    <mergeCell ref="A13:A17"/>
-    <mergeCell ref="B13:B17"/>
-    <mergeCell ref="C13:C17"/>
-    <mergeCell ref="G13:G17"/>
-    <mergeCell ref="I13:I17"/>
-    <mergeCell ref="A18:A19"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="C18:C19"/>
-    <mergeCell ref="G18:G19"/>
-    <mergeCell ref="I18:I19"/>
-    <mergeCell ref="C21:C27"/>
-    <mergeCell ref="B21:B27"/>
-    <mergeCell ref="A21:A27"/>
-    <mergeCell ref="G21:G27"/>
-    <mergeCell ref="I21:I27"/>
-    <mergeCell ref="C28:C31"/>
-    <mergeCell ref="B28:B31"/>
-    <mergeCell ref="A28:A31"/>
-    <mergeCell ref="G28:G31"/>
-    <mergeCell ref="I28:I31"/>
-    <mergeCell ref="A32:A34"/>
-    <mergeCell ref="B32:B34"/>
-    <mergeCell ref="C32:C34"/>
-    <mergeCell ref="G32:G34"/>
-    <mergeCell ref="I32:I34"/>
-    <mergeCell ref="A35:A36"/>
-    <mergeCell ref="B35:B36"/>
-    <mergeCell ref="C35:C36"/>
-    <mergeCell ref="G35:G36"/>
-    <mergeCell ref="I35:I36"/>
-    <mergeCell ref="A39:A40"/>
-    <mergeCell ref="B39:B40"/>
-    <mergeCell ref="C39:C40"/>
-    <mergeCell ref="G39:G40"/>
-    <mergeCell ref="I39:I40"/>
   </mergeCells>
   <phoneticPr fontId="9" type="noConversion"/>
   <pageMargins left="0.75000000000000011" right="0.75000000000000011" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" scale="59" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="100"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>